<commit_message>
construction / initialization memanager
</commit_message>
<xml_diff>
--- a/memory_manager/doc/memanager_construct_checker.xlsx
+++ b/memory_manager/doc/memanager_construct_checker.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>start</t>
+  </si>
   <si>
     <t>jump</t>
   </si>
@@ -34,10 +37,10 @@
     <t>chunk_size</t>
   </si>
   <si>
+    <t>&lt;</t>
+  </si>
+  <si>
     <t>min_chunk_size</t>
-  </si>
-  <si>
-    <t>&lt;</t>
   </si>
 </sst>
 </file>
@@ -70,22 +73,28 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -310,82 +319,91 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="2">
+        <f>32</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>16.0</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+    </row>
+    <row r="3">
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
         <v>256.0</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3">
-        <f>FLoor(D3/3)</f>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <f>FLoor(D4/3)</f>
         <v>682</v>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
+    <row r="4">
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
         <v>2048.0</v>
       </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4">
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <f>3*D2</f>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <f>3*D3</f>
         <v>768</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5">
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
         <v>262144.0</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6">
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3">
-        <f>D2*(D2+1)/2+(D1*(D2+1))+(D3-D2)*(D1+1)</f>
-        <v>67472</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <f>(1/2*D3)*(D3-1)+D1+D4*(D2+1)</f>
+        <v>67488</v>
+      </c>
     </row>
     <row r="7">
-      <c r="D7" s="3">
-        <f>(1/2*D2)*(D2-1)+D1+D3*(D1+1)</f>
-        <v>67472</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="D9" s="3">
-        <f>D5-D1-D3-D3*D1</f>
-        <v>227312</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2">
+        <f>D3*(D3+1)/2+(D2*D3)+D1+(D4-D3)*(D2+1)</f>
+        <v>67488</v>
+      </c>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="10">
+      <c r="D10" s="2">
+        <f>D6-D1-D4-D4*D2</f>
+        <v>227296</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1">
-        <f>(D2-1)*D2/2</f>
+      <c r="F10" s="1">
+        <f>(D3-1)*D3/2</f>
         <v>32640</v>
       </c>
     </row>

</xml_diff>